<commit_message>
Updated the TimeDurationComparison.xlsx with proper time duration outputs for the Matplotlib plot.
</commit_message>
<xml_diff>
--- a/TimeDurationComparison.xlsx
+++ b/TimeDurationComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\SortProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAC766A-307C-4D07-B624-23002FE60BC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A168CE53-5B52-4D43-99FD-6D42D09D8A1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19755" yWindow="0" windowWidth="17265" windowHeight="10800" xr2:uid="{432D40FB-5E15-486E-A46E-98D79B6ED7BD}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +424,10 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1.0025501251220701E-3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.99723243713378E-3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -438,13 +438,13 @@
         <v>1000</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>6.0007572174072196E-3</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.133010864257812</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.0008811950683501E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,13 +452,13 @@
         <v>10000</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>7.0005416870117104E-2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.135011911392211</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>9.0003013610839792E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,13 +466,13 @@
         <v>100000</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.90207433700561501</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.20201754570007299</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>6.8008661270141602E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>